<commit_message>
close #260: Add verification for child levels in composition hierarchy and bump version to 0.5.03
</commit_message>
<xml_diff>
--- a/input_data/data_errors_16/descricao.xlsx
+++ b/input_data/data_errors_16/descricao.xlsx
@@ -510,10 +510,10 @@
   </sheetPr>
   <dimension ref="A1:Y866"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.61328125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -962,7 +962,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="7" t="n">
-        <v>5</v>
+        <v>200</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>49</v>

</xml_diff>